<commit_message>
updating Task 3: Event-driven validation and lag-aware impact modeling
</commit_message>
<xml_diff>
--- a/data/processed/task3_event_impact_matrix.xlsx
+++ b/data/processed/task3_event_impact_matrix.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>National Digital Payments Strategy (NDPS) 2026-2030 Launch</t>
+          <t>NDPS 2026-2030 Launch</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Instant Payment System (IPS / Ethiopay) Launch</t>
+          <t>IPS / Ethiopay Launch</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -782,7 +782,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>National Digital Payments Strategy (NDPS) 2026-2030 Launch</t>
+          <t>NDPS 2026-2030 Launch</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -802,7 +802,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Instant Payment System (IPS / Ethiopay) Launch</t>
+          <t>IPS / Ethiopay Launch</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">

</xml_diff>

<commit_message>
Task 4: Sparse-safe forecasting – extrapolation, uncertainty bands, plots & summary table (2025–2027)
</commit_message>
<xml_diff>
--- a/data/processed/task3_event_impact_matrix.xlsx
+++ b/data/processed/task3_event_impact_matrix.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>National Digital Payments Strategy (NDPS) 2026-2030 Launch</t>
+          <t>NDPS 2026-2030 Launch</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Instant Payment System (IPS / Ethiopay) Launch</t>
+          <t>IPS / Ethiopay Launch</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -782,7 +782,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>National Digital Payments Strategy (NDPS) 2026-2030 Launch</t>
+          <t>NDPS 2026-2030 Launch</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -802,7 +802,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Instant Payment System (IPS / Ethiopay) Launch</t>
+          <t>IPS / Ethiopay Launch</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">

</xml_diff>